<commit_message>
getting swim to converge and simulate Chloride
</commit_message>
<xml_diff>
--- a/Tests/Validation/System/Hudson/observed.xlsx
+++ b/Tests/Validation/System/Hudson/observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Tests\Validation\System\Hudson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6DD0FD-58D4-43D5-93E5-273D5BF1B116}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA9551E-C643-4AF9-9E00-14A454B36503}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="8652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="8652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ObservedCrop" sheetId="2" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="80">
   <si>
     <t>Cl(1)</t>
   </si>
@@ -375,6 +375,15 @@
   <si>
     <t>W1</t>
   </si>
+  <si>
+    <t>Cl110</t>
+  </si>
+  <si>
+    <t>Cl210</t>
+  </si>
+  <si>
+    <t>Cl310</t>
+  </si>
 </sst>
 </file>
 
@@ -413,7 +422,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -421,15 +430,105 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,7 +811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1141,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1577,744 +1676,898 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="16.5234375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>76</v>
       </c>
       <c r="B2" s="2">
         <v>34578</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
+        <f>SUM(F2:K2)</f>
+        <v>159.21010376443058</v>
+      </c>
+      <c r="D2" s="4">
+        <f>SUM(L2:P2)</f>
+        <v>1430.1202200047887</v>
+      </c>
+      <c r="E2" s="4">
+        <f>SUM(Q2:U2)</f>
+        <v>3284.5383796132237</v>
+      </c>
+      <c r="F2" s="5">
         <v>13.75</v>
       </c>
-      <c r="D2">
-        <v>15.5413645</v>
-      </c>
-      <c r="E2">
-        <v>11.99760657</v>
-      </c>
-      <c r="F2">
-        <v>12.450416110000001</v>
-      </c>
-      <c r="G2">
-        <v>11.93948441</v>
-      </c>
-      <c r="H2">
-        <v>13.00691095</v>
-      </c>
-      <c r="I2">
-        <v>30.708216499999999</v>
-      </c>
-      <c r="J2">
-        <v>64.677080349999997</v>
-      </c>
-      <c r="K2">
-        <v>119.8512077</v>
-      </c>
-      <c r="L2">
-        <v>168.338381</v>
-      </c>
-      <c r="M2">
-        <v>212.3085394</v>
-      </c>
-      <c r="N2">
-        <v>248.51476790000001</v>
-      </c>
-      <c r="O2">
-        <v>268.15979060000001</v>
-      </c>
-      <c r="P2">
-        <v>264.50170659999998</v>
-      </c>
-      <c r="Q2">
-        <v>262.57601340000002</v>
-      </c>
-      <c r="R2">
-        <v>238.64823419999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="G2" s="6">
+        <v>34.191001903457362</v>
+      </c>
+      <c r="H2" s="6">
+        <v>26.394734452350477</v>
+      </c>
+      <c r="I2" s="6">
+        <v>27.390915440026966</v>
+      </c>
+      <c r="J2" s="6">
+        <v>26.266865697129493</v>
+      </c>
+      <c r="K2" s="6">
+        <v>31.216586271466284</v>
+      </c>
+      <c r="L2" s="6">
+        <v>73.699719598109525</v>
+      </c>
+      <c r="M2" s="6">
+        <v>155.22499283951043</v>
+      </c>
+      <c r="N2" s="6">
+        <v>287.64289859075222</v>
+      </c>
+      <c r="O2" s="6">
+        <v>404.01211451724498</v>
+      </c>
+      <c r="P2" s="6">
+        <v>509.54049445917144</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>596.43544290107229</v>
+      </c>
+      <c r="R2" s="6">
+        <v>697.21545548725294</v>
+      </c>
+      <c r="S2" s="6">
+        <v>687.70443728806447</v>
+      </c>
+      <c r="T2" s="6">
+        <v>682.69763492614129</v>
+      </c>
+      <c r="U2" s="7">
+        <v>620.48540901069282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>76</v>
       </c>
       <c r="B3" s="2">
         <v>34790</v>
       </c>
-      <c r="C3">
-        <v>6.5674999999999999</v>
-      </c>
-      <c r="D3">
-        <v>6.7060198</v>
-      </c>
-      <c r="E3">
-        <v>6.6372955429999996</v>
-      </c>
-      <c r="F3">
-        <v>7.5282678860000001</v>
-      </c>
-      <c r="G3">
-        <v>8.9597520589999995</v>
-      </c>
-      <c r="H3">
-        <v>13.25403697</v>
-      </c>
-      <c r="I3">
-        <v>31.105580400000001</v>
-      </c>
-      <c r="J3">
-        <v>68.808071960000007</v>
-      </c>
-      <c r="K3">
-        <v>125.51387990000001</v>
-      </c>
-      <c r="L3">
-        <v>189.8830706</v>
-      </c>
-      <c r="M3">
-        <v>240.90359749999999</v>
-      </c>
-      <c r="N3">
-        <v>270.42237390000003</v>
-      </c>
-      <c r="O3">
-        <v>285.68442679999998</v>
-      </c>
-      <c r="P3">
-        <v>282.3903047</v>
-      </c>
-      <c r="Q3">
-        <v>267.55238709999998</v>
-      </c>
-      <c r="R3">
-        <v>250.57786569999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:C13" si="0">SUM(F3:K3)</f>
+        <v>104.00612637072592</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D13" si="1">SUM(L3:P3)</f>
+        <v>1574.9140806823295</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:E13" si="2">SUM(Q3:U3)</f>
+        <v>3473.1466564220973</v>
+      </c>
+      <c r="F3" s="8">
+        <v>6.567499999999999</v>
+      </c>
+      <c r="G3" s="9">
+        <v>14.753243560830773</v>
+      </c>
+      <c r="H3" s="9">
+        <v>14.602050194250957</v>
+      </c>
+      <c r="I3" s="9">
+        <v>16.562189348231101</v>
+      </c>
+      <c r="J3" s="9">
+        <v>19.711454530537686</v>
+      </c>
+      <c r="K3" s="9">
+        <v>31.809688736875412</v>
+      </c>
+      <c r="L3" s="9">
+        <v>74.653392963246674</v>
+      </c>
+      <c r="M3" s="9">
+        <v>165.13937269474624</v>
+      </c>
+      <c r="N3" s="9">
+        <v>301.23331165033693</v>
+      </c>
+      <c r="O3" s="9">
+        <v>455.7193693617827</v>
+      </c>
+      <c r="P3" s="9">
+        <v>578.16863401221701</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>649.01369734522336</v>
+      </c>
+      <c r="R3" s="9">
+        <v>742.77950960939472</v>
+      </c>
+      <c r="S3" s="9">
+        <v>734.21479209197571</v>
+      </c>
+      <c r="T3" s="9">
+        <v>695.63620647478024</v>
+      </c>
+      <c r="U3" s="10">
+        <v>651.50245090072349</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>76</v>
       </c>
       <c r="B4" s="2">
         <v>35004</v>
       </c>
-      <c r="C4">
-        <v>23.322500000000002</v>
-      </c>
-      <c r="D4">
-        <v>27.025647240000001</v>
-      </c>
-      <c r="E4">
-        <v>21.998252480000001</v>
-      </c>
-      <c r="F4">
-        <v>19.367653860000001</v>
-      </c>
-      <c r="G4">
-        <v>17.618865589999999</v>
-      </c>
-      <c r="H4">
-        <v>16.167377810000001</v>
-      </c>
-      <c r="I4">
-        <v>21.65245753</v>
-      </c>
-      <c r="J4">
-        <v>49.727724379999998</v>
-      </c>
-      <c r="K4">
-        <v>95.632376320000006</v>
-      </c>
-      <c r="L4">
-        <v>155.2204103</v>
-      </c>
-      <c r="M4">
-        <v>213.3536402</v>
-      </c>
-      <c r="N4">
-        <v>261.60381660000002</v>
-      </c>
-      <c r="O4">
-        <v>296.22593999999998</v>
-      </c>
-      <c r="P4">
-        <v>316.78103060000001</v>
-      </c>
-      <c r="Q4">
-        <v>312.77060840000001</v>
-      </c>
-      <c r="R4">
-        <v>289.85484789999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" s="4">
+        <f t="shared" si="0"/>
+        <v>251.34712890813802</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="1"/>
+        <v>1285.4078610687457</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="2"/>
+        <v>3788.493469954492</v>
+      </c>
+      <c r="F4" s="8">
+        <v>23.322499999999998</v>
+      </c>
+      <c r="G4" s="9">
+        <v>59.456423932271392</v>
+      </c>
+      <c r="H4" s="9">
+        <v>48.396155450811719</v>
+      </c>
+      <c r="I4" s="9">
+        <v>42.608838483163588</v>
+      </c>
+      <c r="J4" s="9">
+        <v>38.76150428937359</v>
+      </c>
+      <c r="K4" s="9">
+        <v>38.801706752517717</v>
+      </c>
+      <c r="L4" s="9">
+        <v>51.965898083235544</v>
+      </c>
+      <c r="M4" s="9">
+        <v>119.34653850244825</v>
+      </c>
+      <c r="N4" s="9">
+        <v>229.51770317343704</v>
+      </c>
+      <c r="O4" s="9">
+        <v>372.52898481698674</v>
+      </c>
+      <c r="P4" s="9">
+        <v>512.048736492638</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>627.84915974353407</v>
+      </c>
+      <c r="R4" s="9">
+        <v>770.18744410969271</v>
+      </c>
+      <c r="S4" s="9">
+        <v>823.63067955668521</v>
+      </c>
+      <c r="T4" s="9">
+        <v>813.20358187784029</v>
+      </c>
+      <c r="U4" s="10">
+        <v>753.62260466673979</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>76</v>
       </c>
       <c r="B5" s="2">
         <v>35156</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
+        <v>187.42970617451022</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="1"/>
+        <v>1460.5176894091214</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="2"/>
+        <v>3548.1879491060572</v>
+      </c>
+      <c r="F5" s="8">
         <v>34.002499999999998</v>
       </c>
-      <c r="D5">
-        <v>11.489771019999999</v>
-      </c>
-      <c r="E5">
-        <v>11.85154781</v>
-      </c>
-      <c r="F5">
-        <v>13.1735729</v>
-      </c>
-      <c r="G5">
-        <v>15.55664232</v>
-      </c>
-      <c r="H5">
-        <v>16.195763029999998</v>
-      </c>
-      <c r="I5">
-        <v>28.275051479999998</v>
-      </c>
-      <c r="J5">
-        <v>62.164886770000003</v>
-      </c>
-      <c r="K5">
-        <v>116.0326957</v>
-      </c>
-      <c r="L5">
-        <v>172.7066647</v>
-      </c>
-      <c r="M5">
-        <v>229.3697387</v>
-      </c>
-      <c r="N5">
-        <v>271.24466580000001</v>
-      </c>
-      <c r="O5">
-        <v>290.21350569999998</v>
-      </c>
-      <c r="P5">
-        <v>295.67279550000001</v>
-      </c>
-      <c r="Q5">
-        <v>278.19521359999999</v>
-      </c>
-      <c r="R5">
-        <v>250.22646639999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="G5" s="9">
+        <v>25.277496239363575</v>
+      </c>
+      <c r="H5" s="9">
+        <v>26.07340517606244</v>
+      </c>
+      <c r="I5" s="9">
+        <v>28.981860385646673</v>
+      </c>
+      <c r="J5" s="9">
+        <v>34.22461309817065</v>
+      </c>
+      <c r="K5" s="9">
+        <v>38.869831275266904</v>
+      </c>
+      <c r="L5" s="9">
+        <v>67.860123542774772</v>
+      </c>
+      <c r="M5" s="9">
+        <v>149.19572824927474</v>
+      </c>
+      <c r="N5" s="9">
+        <v>278.47846962566706</v>
+      </c>
+      <c r="O5" s="9">
+        <v>414.49599520303326</v>
+      </c>
+      <c r="P5" s="9">
+        <v>550.48737278837154</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>650.98719802512755</v>
+      </c>
+      <c r="R5" s="9">
+        <v>754.55511480160692</v>
+      </c>
+      <c r="S5" s="9">
+        <v>768.74926817894368</v>
+      </c>
+      <c r="T5" s="9">
+        <v>723.30755533454226</v>
+      </c>
+      <c r="U5" s="10">
+        <v>650.58881276583713</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>76</v>
       </c>
       <c r="B6" s="2">
         <v>35370</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>131.16063025324803</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="1"/>
+        <v>967.89426739727935</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="2"/>
+        <v>3010.9352419939469</v>
+      </c>
+      <c r="F6" s="8">
         <v>11.39875</v>
       </c>
-      <c r="D6">
-        <v>12.48579468</v>
-      </c>
-      <c r="E6">
-        <v>12.52660981</v>
-      </c>
-      <c r="F6">
-        <v>12.287846200000001</v>
-      </c>
-      <c r="G6">
-        <v>8.0732845080000004</v>
-      </c>
-      <c r="H6">
-        <v>8.3083761710000008</v>
-      </c>
-      <c r="I6">
-        <v>14.61450447</v>
-      </c>
-      <c r="J6">
-        <v>34.70000022</v>
-      </c>
-      <c r="K6">
-        <v>71.272853589999997</v>
-      </c>
-      <c r="L6">
-        <v>121.0148437</v>
-      </c>
-      <c r="M6">
-        <v>161.68707610000001</v>
-      </c>
-      <c r="N6">
-        <v>214.68685289999999</v>
-      </c>
-      <c r="O6">
-        <v>232.4117072</v>
-      </c>
-      <c r="P6">
-        <v>246.1065328</v>
-      </c>
-      <c r="Q6">
-        <v>248.24888089999999</v>
-      </c>
-      <c r="R6">
-        <v>233.11241559999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" s="9">
+        <v>27.468748295547055</v>
+      </c>
+      <c r="H6" s="9">
+        <v>27.558541584960285</v>
+      </c>
+      <c r="I6" s="9">
+        <v>27.033261643246796</v>
+      </c>
+      <c r="J6" s="9">
+        <v>17.761225918687167</v>
+      </c>
+      <c r="K6" s="9">
+        <v>19.940102810806735</v>
+      </c>
+      <c r="L6" s="9">
+        <v>35.074810739215422</v>
+      </c>
+      <c r="M6" s="9">
+        <v>83.280000522235127</v>
+      </c>
+      <c r="N6" s="9">
+        <v>171.05484862526134</v>
+      </c>
+      <c r="O6" s="9">
+        <v>290.43562484131854</v>
+      </c>
+      <c r="P6" s="9">
+        <v>388.04898266924886</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>515.24844698388881</v>
+      </c>
+      <c r="R6" s="9">
+        <v>604.27043877076369</v>
+      </c>
+      <c r="S6" s="9">
+        <v>639.87698539129917</v>
+      </c>
+      <c r="T6" s="9">
+        <v>645.44709023059818</v>
+      </c>
+      <c r="U6" s="10">
+        <v>606.09228061739691</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>76</v>
       </c>
       <c r="B7" s="2">
         <v>35521</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>244.17473923871307</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="1"/>
+        <v>1944.6289483207415</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="2"/>
+        <v>4137.76935320546</v>
+      </c>
+      <c r="F7" s="8">
         <v>22.23</v>
       </c>
-      <c r="D7">
-        <v>18.896315269999999</v>
-      </c>
-      <c r="E7">
-        <v>19.879391420000001</v>
-      </c>
-      <c r="F7">
-        <v>19.74896815</v>
-      </c>
-      <c r="G7">
-        <v>20.527927439999999</v>
-      </c>
-      <c r="H7">
-        <v>20.012089270000001</v>
-      </c>
-      <c r="I7">
-        <v>33.667573470000001</v>
-      </c>
-      <c r="J7">
-        <v>83.553399839999997</v>
-      </c>
-      <c r="K7">
-        <v>163.1620331</v>
-      </c>
-      <c r="L7">
-        <v>238.973231</v>
-      </c>
-      <c r="M7">
-        <v>290.90582439999997</v>
-      </c>
-      <c r="N7">
-        <v>312.55350579999998</v>
-      </c>
-      <c r="O7">
-        <v>321.24393120000002</v>
-      </c>
-      <c r="P7">
-        <v>324.14727040000002</v>
-      </c>
-      <c r="Q7">
-        <v>343.42707919999998</v>
-      </c>
-      <c r="R7">
-        <v>314.120542</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="G7" s="9">
+        <v>41.571893588914726</v>
+      </c>
+      <c r="H7" s="9">
+        <v>43.734661113329906</v>
+      </c>
+      <c r="I7" s="9">
+        <v>43.447729933462277</v>
+      </c>
+      <c r="J7" s="9">
+        <v>45.161440360969095</v>
+      </c>
+      <c r="K7" s="9">
+        <v>48.029014242037071</v>
+      </c>
+      <c r="L7" s="9">
+        <v>80.802176318720868</v>
+      </c>
+      <c r="M7" s="9">
+        <v>200.52815961181636</v>
+      </c>
+      <c r="N7" s="9">
+        <v>391.58887940214095</v>
+      </c>
+      <c r="O7" s="9">
+        <v>573.53575435424057</v>
+      </c>
+      <c r="P7" s="9">
+        <v>698.17397863382291</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>750.1284138977685</v>
+      </c>
+      <c r="R7" s="9">
+        <v>835.23422121866042</v>
+      </c>
+      <c r="S7" s="9">
+        <v>842.78290304931716</v>
+      </c>
+      <c r="T7" s="9">
+        <v>892.91040594684637</v>
+      </c>
+      <c r="U7" s="10">
+        <v>816.71340909286721</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>76</v>
       </c>
       <c r="B8" s="2">
         <v>35735</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>114.88109839650724</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="1"/>
+        <v>1663.0780781557257</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="2"/>
+        <v>3534.0719302127777</v>
+      </c>
+      <c r="F8" s="8">
         <v>19.453749999999999</v>
       </c>
-      <c r="D8">
-        <v>10.811291860000001</v>
-      </c>
-      <c r="E8">
-        <v>6.0610406440000002</v>
-      </c>
-      <c r="F8">
-        <v>5.5284312059999996</v>
-      </c>
-      <c r="G8">
-        <v>6.6644347420000001</v>
-      </c>
-      <c r="H8">
-        <v>13.11829659</v>
-      </c>
-      <c r="I8">
-        <v>37.067594270000001</v>
-      </c>
-      <c r="J8">
-        <v>81.710076490000006</v>
-      </c>
-      <c r="K8">
-        <v>138.8852952</v>
-      </c>
-      <c r="L8">
-        <v>195.0125261</v>
-      </c>
-      <c r="M8">
-        <v>240.2737071</v>
-      </c>
-      <c r="N8">
-        <v>268.71580890000001</v>
-      </c>
-      <c r="O8">
-        <v>277.27861300000001</v>
-      </c>
-      <c r="P8">
-        <v>280.98173489999999</v>
-      </c>
-      <c r="Q8">
-        <v>281.83296639999998</v>
-      </c>
-      <c r="R8">
-        <v>271.1197583</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="G8" s="9">
+        <v>23.784842084482612</v>
+      </c>
+      <c r="H8" s="9">
+        <v>13.334289416890011</v>
+      </c>
+      <c r="I8" s="9">
+        <v>12.162548653423357</v>
+      </c>
+      <c r="J8" s="9">
+        <v>14.661756432133</v>
+      </c>
+      <c r="K8" s="9">
+        <v>31.483911809578256</v>
+      </c>
+      <c r="L8" s="9">
+        <v>88.962226250679592</v>
+      </c>
+      <c r="M8" s="9">
+        <v>196.10418356420595</v>
+      </c>
+      <c r="N8" s="9">
+        <v>333.32470858714601</v>
+      </c>
+      <c r="O8" s="9">
+        <v>468.03006274934972</v>
+      </c>
+      <c r="P8" s="9">
+        <v>576.6568970043445</v>
+      </c>
+      <c r="Q8" s="9">
+        <v>644.91794140737409</v>
+      </c>
+      <c r="R8" s="9">
+        <v>720.92439385168177</v>
+      </c>
+      <c r="S8" s="9">
+        <v>730.5525106465609</v>
+      </c>
+      <c r="T8" s="9">
+        <v>732.76571275103186</v>
+      </c>
+      <c r="U8" s="10">
+        <v>704.91137155612921</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>76</v>
       </c>
       <c r="B9" s="2">
         <v>35916</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>63.242769274498826</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="1"/>
+        <v>1241.2591987086287</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="2"/>
+        <v>4381.5153557175581</v>
+      </c>
+      <c r="F9" s="8">
         <v>8.3887499999999999</v>
       </c>
-      <c r="D9">
-        <v>2.6621844029999999</v>
-      </c>
-      <c r="E9">
-        <v>6.6743644069999997</v>
-      </c>
-      <c r="F9">
-        <v>6.4029567329999999</v>
-      </c>
-      <c r="G9">
-        <v>7.4547537579999998</v>
-      </c>
-      <c r="H9">
-        <v>1.5944370059999999</v>
-      </c>
-      <c r="I9">
-        <v>4.9033869670000003</v>
-      </c>
-      <c r="J9">
-        <v>27.113477769999999</v>
-      </c>
-      <c r="K9">
-        <v>75.973188750000006</v>
-      </c>
-      <c r="L9">
-        <v>157.49463750000001</v>
-      </c>
-      <c r="M9">
-        <v>251.7066418</v>
-      </c>
-      <c r="N9">
-        <v>309.83903379999998</v>
-      </c>
-      <c r="O9">
-        <v>338.7074733</v>
-      </c>
-      <c r="P9">
-        <v>347.42341599999997</v>
-      </c>
-      <c r="Q9">
-        <v>358.38387280000001</v>
-      </c>
-      <c r="R9">
-        <v>354.67818970000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="G9" s="9">
+        <v>5.8568056874230381</v>
+      </c>
+      <c r="H9" s="9">
+        <v>14.683601694409523</v>
+      </c>
+      <c r="I9" s="9">
+        <v>14.086504811520102</v>
+      </c>
+      <c r="J9" s="9">
+        <v>16.400458267300937</v>
+      </c>
+      <c r="K9" s="9">
+        <v>3.8266488138452273</v>
+      </c>
+      <c r="L9" s="9">
+        <v>11.768128720903922</v>
+      </c>
+      <c r="M9" s="9">
+        <v>65.072346653375675</v>
+      </c>
+      <c r="N9" s="9">
+        <v>182.33565299373294</v>
+      </c>
+      <c r="O9" s="9">
+        <v>377.98712993934447</v>
+      </c>
+      <c r="P9" s="9">
+        <v>604.09594040127172</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>743.61368104961332</v>
+      </c>
+      <c r="R9" s="9">
+        <v>880.63943064207444</v>
+      </c>
+      <c r="S9" s="9">
+        <v>903.3008814873001</v>
+      </c>
+      <c r="T9" s="9">
+        <v>931.79806937116052</v>
+      </c>
+      <c r="U9" s="10">
+        <v>922.16329316740951</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>76</v>
       </c>
       <c r="B10" s="2">
         <v>36100</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>168.89229575188483</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="1"/>
+        <v>1229.9094679818445</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="2"/>
+        <v>3874.06844483021</v>
+      </c>
+      <c r="F10" s="8">
         <v>17.271249999999998</v>
       </c>
-      <c r="D10">
-        <v>12.18463249</v>
-      </c>
-      <c r="E10">
-        <v>14.30238653</v>
-      </c>
-      <c r="F10">
-        <v>11.714985029999999</v>
-      </c>
-      <c r="G10">
-        <v>13.961501999999999</v>
-      </c>
-      <c r="H10">
-        <v>15.358888520000001</v>
-      </c>
-      <c r="I10">
-        <v>19.201742410000001</v>
-      </c>
-      <c r="J10">
-        <v>29.287347669999999</v>
-      </c>
-      <c r="K10">
-        <v>70.642186670000001</v>
-      </c>
-      <c r="L10">
-        <v>157.52082429999999</v>
-      </c>
-      <c r="M10">
-        <v>235.81017729999999</v>
-      </c>
-      <c r="N10">
-        <v>285.03145699999999</v>
-      </c>
-      <c r="O10">
-        <v>307.43184189999999</v>
-      </c>
-      <c r="P10">
-        <v>316.8785767</v>
-      </c>
-      <c r="Q10">
-        <v>303.8996636</v>
-      </c>
-      <c r="R10">
-        <v>298.71028239999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="G10" s="9">
+        <v>26.806191482304087</v>
+      </c>
+      <c r="H10" s="9">
+        <v>31.465250372217806</v>
+      </c>
+      <c r="I10" s="9">
+        <v>25.772967069634358</v>
+      </c>
+      <c r="J10" s="9">
+        <v>30.715304389757115</v>
+      </c>
+      <c r="K10" s="9">
+        <v>36.861332437971477</v>
+      </c>
+      <c r="L10" s="9">
+        <v>46.084181786700725</v>
+      </c>
+      <c r="M10" s="9">
+        <v>70.289634419020999</v>
+      </c>
+      <c r="N10" s="9">
+        <v>169.54124801816255</v>
+      </c>
+      <c r="O10" s="9">
+        <v>378.04997829105946</v>
+      </c>
+      <c r="P10" s="9">
+        <v>565.94442546690095</v>
+      </c>
+      <c r="Q10" s="9">
+        <v>684.07549682957392</v>
+      </c>
+      <c r="R10" s="9">
+        <v>799.32278884809796</v>
+      </c>
+      <c r="S10" s="9">
+        <v>823.88429936600596</v>
+      </c>
+      <c r="T10" s="9">
+        <v>790.13912548001053</v>
+      </c>
+      <c r="U10" s="10">
+        <v>776.64673430652169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>76</v>
       </c>
       <c r="B11" s="2">
         <v>36312</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
+        <v>126.50508601281143</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="1"/>
+        <v>519.09450808430495</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="2"/>
+        <v>3420.4218968267578</v>
+      </c>
+      <c r="F11" s="8">
         <v>10.895</v>
       </c>
-      <c r="D11">
-        <v>8.7502595509999992</v>
-      </c>
-      <c r="E11">
-        <v>9.1302689790000002</v>
-      </c>
-      <c r="F11">
-        <v>10.26865016</v>
-      </c>
-      <c r="G11">
-        <v>10.64313091</v>
-      </c>
-      <c r="H11">
-        <v>12.61125204</v>
-      </c>
-      <c r="I11">
-        <v>19.25542883</v>
-      </c>
-      <c r="J11">
-        <v>25.27869862</v>
-      </c>
-      <c r="K11">
-        <v>39.617221319999999</v>
-      </c>
-      <c r="L11">
-        <v>48.658112680000002</v>
-      </c>
-      <c r="M11">
-        <v>83.479916919999994</v>
-      </c>
-      <c r="N11">
-        <v>145.5617421</v>
-      </c>
-      <c r="O11">
-        <v>212.41632519999999</v>
-      </c>
-      <c r="P11">
-        <v>254.60247609999999</v>
-      </c>
-      <c r="Q11">
-        <v>336.64068370000001</v>
-      </c>
-      <c r="R11">
-        <v>377.52271330000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="G11" s="9">
+        <v>19.250571012914037</v>
+      </c>
+      <c r="H11" s="9">
+        <v>20.086591753268539</v>
+      </c>
+      <c r="I11" s="9">
+        <v>22.591030355369462</v>
+      </c>
+      <c r="J11" s="9">
+        <v>23.414888002069347</v>
+      </c>
+      <c r="K11" s="9">
+        <v>30.267004889190044</v>
+      </c>
+      <c r="L11" s="9">
+        <v>46.213029188865193</v>
+      </c>
+      <c r="M11" s="9">
+        <v>60.668876695966105</v>
+      </c>
+      <c r="N11" s="9">
+        <v>95.081331177125691</v>
+      </c>
+      <c r="O11" s="9">
+        <v>116.77947042201062</v>
+      </c>
+      <c r="P11" s="9">
+        <v>200.35180060033733</v>
+      </c>
+      <c r="Q11" s="9">
+        <v>349.34818108104406</v>
+      </c>
+      <c r="R11" s="9">
+        <v>552.2824456033278</v>
+      </c>
+      <c r="S11" s="9">
+        <v>661.96643794157092</v>
+      </c>
+      <c r="T11" s="9">
+        <v>875.26577750781303</v>
+      </c>
+      <c r="U11" s="10">
+        <v>981.55905469300171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>76</v>
       </c>
       <c r="B12" s="2">
         <v>36465</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
+        <f t="shared" si="0"/>
+        <v>72.119482620682177</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="1"/>
+        <v>387.10830246209423</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="2"/>
+        <v>3512.2754724011265</v>
+      </c>
+      <c r="F12" s="8">
         <v>12.21</v>
       </c>
-      <c r="D12">
-        <v>7.4027576450000003</v>
-      </c>
-      <c r="E12">
-        <v>5.1808403009999999</v>
-      </c>
-      <c r="F12">
-        <v>4.583631145</v>
-      </c>
-      <c r="G12">
-        <v>4.6389220990000002</v>
-      </c>
-      <c r="H12">
-        <v>4.9733125009999997</v>
-      </c>
-      <c r="I12">
-        <v>6.6826599680000003</v>
-      </c>
-      <c r="J12">
-        <v>10.124419619999999</v>
-      </c>
-      <c r="K12">
-        <v>17.107084919999998</v>
-      </c>
-      <c r="L12">
-        <v>38.610510499999997</v>
-      </c>
-      <c r="M12">
-        <v>88.770451019999996</v>
-      </c>
-      <c r="N12">
-        <v>158.4112283</v>
-      </c>
-      <c r="O12">
-        <v>240.02356560000001</v>
-      </c>
-      <c r="P12">
-        <v>294.40955910000002</v>
-      </c>
-      <c r="Q12">
-        <v>327.83289769999999</v>
-      </c>
-      <c r="R12">
-        <v>342.38341009999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="G12" s="9">
+        <v>16.286066818726812</v>
+      </c>
+      <c r="H12" s="9">
+        <v>11.397848663227906</v>
+      </c>
+      <c r="I12" s="9">
+        <v>10.083988519790065</v>
+      </c>
+      <c r="J12" s="9">
+        <v>10.205628617112231</v>
+      </c>
+      <c r="K12" s="9">
+        <v>11.935950001825155</v>
+      </c>
+      <c r="L12" s="9">
+        <v>16.038383922120151</v>
+      </c>
+      <c r="M12" s="9">
+        <v>24.298607087825513</v>
+      </c>
+      <c r="N12" s="9">
+        <v>41.057003815729509</v>
+      </c>
+      <c r="O12" s="9">
+        <v>92.665225196238353</v>
+      </c>
+      <c r="P12" s="9">
+        <v>213.04908244018074</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>380.18694803606815</v>
+      </c>
+      <c r="R12" s="9">
+        <v>624.06127044401615</v>
+      </c>
+      <c r="S12" s="9">
+        <v>765.46485368567642</v>
+      </c>
+      <c r="T12" s="9">
+        <v>852.36553396844783</v>
+      </c>
+      <c r="U12" s="10">
+        <v>890.19686626691805</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>76</v>
       </c>
       <c r="B13" s="2">
         <v>36647</v>
       </c>
-      <c r="C13">
-        <v>6.7149999999999999</v>
-      </c>
-      <c r="D13">
-        <v>6.0663380670000002</v>
-      </c>
-      <c r="E13">
-        <v>6.6849546799999997</v>
-      </c>
-      <c r="F13">
-        <v>6.0689655790000003</v>
-      </c>
-      <c r="G13">
-        <v>6.8214722989999999</v>
-      </c>
-      <c r="H13">
-        <v>5.9825332720000004</v>
-      </c>
-      <c r="I13">
-        <v>6.8922071230000004</v>
-      </c>
-      <c r="J13">
-        <v>9.2570514670000001</v>
-      </c>
-      <c r="K13">
-        <v>11.31003104</v>
-      </c>
-      <c r="L13">
-        <v>23.740483950000002</v>
-      </c>
-      <c r="M13">
-        <v>54.944066929999998</v>
-      </c>
-      <c r="N13">
-        <v>99.426459750000006</v>
-      </c>
-      <c r="O13">
-        <v>158.9381521</v>
-      </c>
-      <c r="P13">
-        <v>211.92377540000001</v>
-      </c>
-      <c r="Q13">
-        <v>238.54086469999999</v>
-      </c>
-      <c r="R13">
-        <v>254.8011735</v>
+      <c r="C13" s="4">
+        <f t="shared" si="0"/>
+        <v>77.484887226284812</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="1"/>
+        <v>254.74521722105283</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="2"/>
+        <v>2485.5538140186009</v>
+      </c>
+      <c r="F13" s="11">
+        <v>6.7150000000000007</v>
+      </c>
+      <c r="G13" s="12">
+        <v>13.345943747501387</v>
+      </c>
+      <c r="H13" s="12">
+        <v>14.706900296195323</v>
+      </c>
+      <c r="I13" s="12">
+        <v>13.351724274017492</v>
+      </c>
+      <c r="J13" s="12">
+        <v>15.007239056903066</v>
+      </c>
+      <c r="K13" s="12">
+        <v>14.358079851667535</v>
+      </c>
+      <c r="L13" s="12">
+        <v>16.541297095917937</v>
+      </c>
+      <c r="M13" s="12">
+        <v>22.216923521728578</v>
+      </c>
+      <c r="N13" s="12">
+        <v>27.1440744902978</v>
+      </c>
+      <c r="O13" s="12">
+        <v>56.977161473753469</v>
+      </c>
+      <c r="P13" s="12">
+        <v>131.86576063935505</v>
+      </c>
+      <c r="Q13" s="12">
+        <v>238.62350339411961</v>
+      </c>
+      <c r="R13" s="12">
+        <v>413.23919551664045</v>
+      </c>
+      <c r="S13" s="12">
+        <v>551.0018160366302</v>
+      </c>
+      <c r="T13" s="12">
+        <v>620.20624809619881</v>
+      </c>
+      <c r="U13" s="13">
+        <v>662.48305097501202</v>
       </c>
     </row>
   </sheetData>
@@ -4923,7 +5176,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>

</xml_diff>